<commit_message>
Add function view log
</commit_message>
<xml_diff>
--- a/UploadDataToDatabase/Resources/MQC-PQC_Template.xlsx
+++ b/UploadDataToDatabase/Resources/MQC-PQC_Template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC73FF30-6D14-4C19-8EA1-2242AA27DA4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2BA4FB-4824-46EA-A727-DCBF388B75C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,14 +11,14 @@
     <sheet name="报表" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">报表!$A$1:$AB$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">报表!$A$1:$Z$19</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Results</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -221,20 +221,6 @@
   </si>
   <si>
     <t>Năm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Số lượng rework
-不良数
-Quantity of rework
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tỷ lệ % rework
-不良率 (%)
-Rework rate
-(%)
-</t>
   </si>
 </sst>
 </file>
@@ -384,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -452,65 +438,56 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -851,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC30"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -882,45 +859,43 @@
     <col min="21" max="21" width="8.5546875" style="1" customWidth="1"/>
     <col min="22" max="22" width="13" style="1" customWidth="1"/>
     <col min="23" max="23" width="10" style="1" customWidth="1"/>
-    <col min="24" max="25" width="9.5546875" style="1" customWidth="1"/>
-    <col min="26" max="27" width="12.33203125" style="20" customWidth="1"/>
-    <col min="28" max="28" width="14.5546875" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="9" style="1"/>
+    <col min="24" max="24" width="9.5546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" style="20" customWidth="1"/>
+    <col min="26" max="26" width="14.5546875" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="159.75" customHeight="1">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:26" ht="159.75" customHeight="1">
+      <c r="A1" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-    </row>
-    <row r="2" spans="1:28" ht="61.2" customHeight="1">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+    </row>
+    <row r="2" spans="1:26" ht="61.2" customHeight="1">
       <c r="A2" s="16"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -951,162 +926,150 @@
       <c r="V2" s="17"/>
       <c r="W2" s="17"/>
       <c r="X2" s="17"/>
-      <c r="Y2" s="23"/>
+      <c r="Y2" s="17"/>
       <c r="Z2" s="17"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="17"/>
-    </row>
-    <row r="3" spans="1:28" ht="27.75" customHeight="1">
-      <c r="A3" s="28" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="27.75" customHeight="1">
+      <c r="A3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="23" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38" t="s">
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
-      <c r="AB3" s="38"/>
-    </row>
-    <row r="4" spans="1:28" ht="34.799999999999997" customHeight="1">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="29" t="s">
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="31"/>
+    </row>
+    <row r="4" spans="1:26" ht="34.799999999999997" customHeight="1">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="24" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="7"/>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="39" t="s">
+      <c r="I4" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="28" t="s">
+      <c r="N4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="29" t="s">
+      <c r="O4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="28" t="s">
+      <c r="P4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="28" t="s">
+      <c r="R4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="S4" s="28" t="s">
+      <c r="S4" s="23" t="s">
         <v>13</v>
       </c>
       <c r="T4" s="7"/>
-      <c r="U4" s="29" t="s">
+      <c r="U4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="V4" s="28" t="s">
+      <c r="V4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="W4" s="28" t="s">
+      <c r="W4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="28" t="s">
+      <c r="X4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="Y4" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z4" s="31" t="s">
+      <c r="Y4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB4" s="28" t="s">
+      <c r="Z4" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="177" customHeight="1">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="42"/>
+    <row r="5" spans="1:26" ht="177" customHeight="1">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="36"/>
       <c r="F5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
       <c r="T5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="U5" s="30"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="32"/>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="29"/>
-    </row>
-    <row r="6" spans="1:28" ht="110.4" customHeight="1">
+      <c r="U5" s="35"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="24"/>
+    </row>
+    <row r="6" spans="1:26" ht="110.4" customHeight="1">
       <c r="A6" s="15"/>
       <c r="B6" s="14"/>
       <c r="C6" s="4"/>
@@ -1131,12 +1094,10 @@
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="4"/>
-    </row>
-    <row r="7" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="4"/>
+    </row>
+    <row r="7" spans="1:26" ht="54.9" customHeight="1">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="4"/>
@@ -1161,12 +1122,10 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="4"/>
-    </row>
-    <row r="8" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="54.9" customHeight="1">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="4"/>
@@ -1191,12 +1150,10 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="4"/>
-    </row>
-    <row r="9" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="4"/>
+    </row>
+    <row r="9" spans="1:26" ht="54.9" customHeight="1">
       <c r="A9" s="15"/>
       <c r="B9" s="15"/>
       <c r="C9" s="4"/>
@@ -1221,12 +1178,10 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="4"/>
-    </row>
-    <row r="10" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="4"/>
+    </row>
+    <row r="10" spans="1:26" ht="54.9" customHeight="1">
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="4"/>
@@ -1251,12 +1206,10 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="4"/>
-    </row>
-    <row r="11" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="4"/>
+    </row>
+    <row r="11" spans="1:26" ht="54.9" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="4"/>
@@ -1281,12 +1234,10 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="4"/>
-    </row>
-    <row r="12" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="4"/>
+    </row>
+    <row r="12" spans="1:26" ht="54.9" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="11"/>
@@ -1311,12 +1262,10 @@
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
       <c r="X12" s="11"/>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="11"/>
-    </row>
-    <row r="13" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="11"/>
+    </row>
+    <row r="13" spans="1:26" ht="54.9" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="11"/>
@@ -1341,12 +1290,10 @@
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
       <c r="X13" s="11"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="11"/>
-    </row>
-    <row r="14" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="11"/>
+    </row>
+    <row r="14" spans="1:26" ht="54.9" customHeight="1">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="11"/>
@@ -1371,12 +1318,10 @@
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
       <c r="X14" s="11"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="11"/>
-    </row>
-    <row r="15" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="11"/>
+    </row>
+    <row r="15" spans="1:26" ht="54.9" customHeight="1">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="11"/>
@@ -1401,12 +1346,10 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
-      <c r="Y15" s="13"/>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="18"/>
-      <c r="AB15" s="11"/>
-    </row>
-    <row r="16" spans="1:28" ht="54.9" customHeight="1">
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="11"/>
+    </row>
+    <row r="16" spans="1:26" ht="54.9" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="11"/>
@@ -1431,12 +1374,10 @@
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
       <c r="X16" s="11"/>
-      <c r="Y16" s="13"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="11"/>
-    </row>
-    <row r="17" spans="1:29" ht="60.75" customHeight="1">
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="11"/>
+    </row>
+    <row r="17" spans="1:27" ht="60.75" customHeight="1">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="11"/>
@@ -1461,80 +1402,74 @@
       <c r="V17" s="11"/>
       <c r="W17" s="11"/>
       <c r="X17" s="11"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="11"/>
-    </row>
-    <row r="18" spans="1:29" ht="96" customHeight="1">
-      <c r="A18" s="34" t="s">
+      <c r="Y17" s="18"/>
+      <c r="Z17" s="11"/>
+    </row>
+    <row r="18" spans="1:27" ht="96" customHeight="1">
+      <c r="A18" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
-      <c r="T18" s="25"/>
-      <c r="U18" s="25"/>
-      <c r="V18" s="25" t="s">
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="W18" s="25"/>
-      <c r="X18" s="26"/>
-      <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="26"/>
-    </row>
-    <row r="19" spans="1:29" ht="30.75" customHeight="1">
-      <c r="A19" s="27" t="s">
+      <c r="W18" s="28"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="22"/>
+    </row>
+    <row r="19" spans="1:27" ht="30.75" customHeight="1">
+      <c r="A19" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="27"/>
-      <c r="Z19" s="27"/>
-      <c r="AA19" s="27"/>
-      <c r="AB19" s="27"/>
-    </row>
-    <row r="21" spans="1:29" ht="54" customHeight="1">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="37"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="37"/>
+      <c r="Z19" s="37"/>
+    </row>
+    <row r="21" spans="1:27" ht="54" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
@@ -1559,293 +1494,277 @@
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
-      <c r="Y21" s="22"/>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="2"/>
-    </row>
-    <row r="22" spans="1:29" ht="56.25" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="26"/>
-    </row>
-    <row r="23" spans="1:29">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
-      <c r="Y23" s="26"/>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="26"/>
-      <c r="AC23" s="26"/>
-    </row>
-    <row r="24" spans="1:29">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
-      <c r="AC24" s="26"/>
-    </row>
-    <row r="25" spans="1:29">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="26"/>
-      <c r="AC25" s="26"/>
-    </row>
-    <row r="26" spans="1:29">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="26"/>
-      <c r="T26" s="26"/>
-      <c r="U26" s="26"/>
-      <c r="V26" s="26"/>
-      <c r="W26" s="26"/>
-      <c r="X26" s="26"/>
-      <c r="Y26" s="26"/>
-      <c r="Z26" s="26"/>
-      <c r="AA26" s="26"/>
-      <c r="AB26" s="26"/>
-      <c r="AC26" s="26"/>
-    </row>
-    <row r="27" spans="1:29">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="26"/>
-      <c r="V27" s="26"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="26"/>
-      <c r="Y27" s="26"/>
-      <c r="Z27" s="26"/>
-      <c r="AA27" s="26"/>
-      <c r="AB27" s="26"/>
-      <c r="AC27" s="26"/>
-    </row>
-    <row r="28" spans="1:29">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="26"/>
-      <c r="V28" s="26"/>
-      <c r="W28" s="26"/>
-      <c r="X28" s="26"/>
-      <c r="Y28" s="26"/>
-      <c r="Z28" s="26"/>
-      <c r="AA28" s="26"/>
-      <c r="AB28" s="26"/>
-      <c r="AC28" s="26"/>
-    </row>
-    <row r="29" spans="1:29">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="26"/>
-      <c r="Z29" s="26"/>
-      <c r="AA29" s="26"/>
-      <c r="AB29" s="26"/>
-      <c r="AC29" s="26"/>
-    </row>
-    <row r="30" spans="1:29">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="26"/>
-      <c r="T30" s="26"/>
-      <c r="U30" s="26"/>
-      <c r="V30" s="26"/>
-      <c r="W30" s="26"/>
-      <c r="X30" s="26"/>
-      <c r="Y30" s="26"/>
-      <c r="Z30" s="26"/>
-      <c r="AA30" s="26"/>
-      <c r="AB30" s="26"/>
-      <c r="AC30" s="26"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="2"/>
+    </row>
+    <row r="22" spans="1:27" ht="56.25" customHeight="1">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+      <c r="V22" s="22"/>
+      <c r="W22" s="22"/>
+      <c r="X22" s="22"/>
+      <c r="Y22" s="22"/>
+      <c r="Z22" s="22"/>
+      <c r="AA22" s="22"/>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
+      <c r="V23" s="22"/>
+      <c r="W23" s="22"/>
+      <c r="X23" s="22"/>
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="22"/>
+      <c r="AA23" s="22"/>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="22"/>
+      <c r="V24" s="22"/>
+      <c r="W24" s="22"/>
+      <c r="X24" s="22"/>
+      <c r="Y24" s="22"/>
+      <c r="Z24" s="22"/>
+      <c r="AA24" s="22"/>
+    </row>
+    <row r="25" spans="1:27">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="22"/>
+      <c r="U25" s="22"/>
+      <c r="V25" s="22"/>
+      <c r="W25" s="22"/>
+      <c r="X25" s="22"/>
+      <c r="Y25" s="22"/>
+      <c r="Z25" s="22"/>
+      <c r="AA25" s="22"/>
+    </row>
+    <row r="26" spans="1:27">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22"/>
+      <c r="Z26" s="22"/>
+      <c r="AA26" s="22"/>
+    </row>
+    <row r="27" spans="1:27">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22"/>
+      <c r="Z27" s="22"/>
+      <c r="AA27" s="22"/>
+    </row>
+    <row r="28" spans="1:27">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22"/>
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+    </row>
+    <row r="29" spans="1:27">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+    </row>
+    <row r="30" spans="1:27">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+      <c r="U30" s="22"/>
+      <c r="V30" s="22"/>
+      <c r="W30" s="22"/>
+      <c r="X30" s="22"/>
+      <c r="Y30" s="22"/>
+      <c r="Z30" s="22"/>
+      <c r="AA30" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="A1:AB1"/>
+  <mergeCells count="35">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N18:U18"/>
+    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="A1:Z1"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="G3:V3"/>
     <mergeCell ref="Q4:Q5"/>
@@ -1854,15 +1773,17 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="W3:AB3"/>
+    <mergeCell ref="W3:Z3"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="U4:U5"/>
-    <mergeCell ref="AA4:AA5"/>
-    <mergeCell ref="A22:AC30"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A22:AA30"/>
     <mergeCell ref="W4:W5"/>
     <mergeCell ref="X4:X5"/>
+    <mergeCell ref="Y4:Y5"/>
     <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="AB4:AB5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="R4:R5"/>
     <mergeCell ref="S4:S5"/>
@@ -1871,17 +1792,9 @@
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:U18"/>
     <mergeCell ref="V18:W18"/>
-    <mergeCell ref="X18:AB18"/>
-    <mergeCell ref="A19:AB19"/>
-    <mergeCell ref="Y4:Y5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="X18:Z18"/>
+    <mergeCell ref="A19:Z19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>